<commit_message>
rename dataset, add plotting result
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaoy\Documents\learning\ETH_master\semester5\科研\constrained smoothing\RTSNet_constrained\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D32CD9-71BD-42EC-BFB4-07FE688095FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91813FD3-EA20-4270-8E45-4C8A9E5B84D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,9 +79,6 @@
     <t>EKF [dB]</t>
   </si>
   <si>
-    <t>Inference Time</t>
-  </si>
-  <si>
     <t>EKF std [dB]</t>
   </si>
   <si>
@@ -95,6 +92,9 @@
   </si>
   <si>
     <t>2) Constrained</t>
+  </si>
+  <si>
+    <t>Inference Time s/traj (colab pro+ CPU)</t>
   </si>
 </sst>
 </file>
@@ -638,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -709,7 +709,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -721,7 +721,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -746,27 +746,29 @@
         <v>-20.6782</v>
       </c>
       <c r="C14" s="19">
-        <f>2.35138511657714/10</f>
-        <v>0.23513851165771399</v>
+        <f>2.12102031707763/10</f>
+        <v>0.21210203170776301</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="28"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="28">
+        <v>0.63129999999999997</v>
+      </c>
       <c r="C15" s="19"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="29">
         <v>-22.6889</v>
       </c>
       <c r="C16" s="22">
-        <f>5.19763970375061/10</f>
-        <v>0.51976397037506106</v>
+        <f>4.10807561874389/10</f>
+        <v>0.41080756187438905</v>
       </c>
       <c r="D16" s="10"/>
     </row>
@@ -774,23 +776,32 @@
       <c r="A17" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="29"/>
+      <c r="B17" s="29">
+        <v>0.89549999999999996</v>
+      </c>
       <c r="C17" s="22"/>
       <c r="D17" s="10"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="24"/>
+        <v>16</v>
+      </c>
+      <c r="B18" s="30">
+        <v>-23.454699999999999</v>
+      </c>
+      <c r="C18" s="24">
+        <f>4.35626101493835/10</f>
+        <v>0.43562610149383502</v>
+      </c>
       <c r="D18" s="10"/>
     </row>
     <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="26"/>
+      <c r="B19" s="26">
+        <v>0.69079999999999997</v>
+      </c>
       <c r="C19" s="32"/>
       <c r="D19" s="10"/>
     </row>
@@ -805,7 +816,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="10"/>
     </row>

</xml_diff>